<commit_message>
✏️ Add more tabs
</commit_message>
<xml_diff>
--- a/export/production_areas.xlsx
+++ b/export/production_areas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -617,11 +617,21 @@
       <c r="F5" t="n">
         <v>807.5</v>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-170</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -755,11 +765,21 @@
       <c r="F9" t="n">
         <v>127.5</v>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-42.5</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -796,6 +816,80 @@
       </c>
       <c r="K10" t="n">
         <v>7291.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>A12</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>51.089</v>
+      </c>
+      <c r="H11" t="n">
+        <v>28</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1100</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2554.45</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>A35</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>18</v>
+      </c>
+      <c r="I12" t="n">
+        <v>100</v>
+      </c>
+      <c r="J12" t="n">
+        <v>50</v>
+      </c>
+      <c r="K12" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>